<commit_message>
Added 3 buttons: Upload clean database, load current results on disk in case of page refresh or problems with last button, delete last entry in case of mistaken number
</commit_message>
<xml_diff>
--- a/App/Data/Results.xlsx
+++ b/App/Data/Results.xlsx
@@ -7,14 +7,21 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="TANDA DAMAS NOVATAS " sheetId="1" r:id="rId1"/>
+    <sheet name="TANDA ÉLITE MASCULINO" sheetId="1" r:id="rId1"/>
+    <sheet name="TANDA SENIOR (19-29 AÑOS)" sheetId="2" r:id="rId2"/>
+    <sheet name="TANDA DAMAS NOVATAS " sheetId="3" r:id="rId3"/>
+    <sheet name="TANDA DAMAS EXPERTAS" sheetId="4" r:id="rId4"/>
+    <sheet name="TANDA MASTER C (50 AÑOS EN ADE" sheetId="5" r:id="rId5"/>
+    <sheet name="TANDA NOVATOS" sheetId="6" r:id="rId6"/>
+    <sheet name="TANDA MASTER B (40-49 AÑOS)" sheetId="7" r:id="rId7"/>
+    <sheet name="TANDA MASTER A (30-39 AÑOS)" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="269">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -37,21 +44,177 @@
     <t>POSICIÓN</t>
   </si>
   <si>
+    <t>Juan Pablo Castaño</t>
+  </si>
+  <si>
+    <t>Juan Camilo Echeverry</t>
+  </si>
+  <si>
+    <t>Juan Manuel Baena</t>
+  </si>
+  <si>
+    <t>TANDA ÉLITE MASCULINO</t>
+  </si>
+  <si>
+    <t>10:22:00</t>
+  </si>
+  <si>
+    <t>10:21:00</t>
+  </si>
+  <si>
+    <t>10:20:00</t>
+  </si>
+  <si>
+    <t>18:05:21.460000</t>
+  </si>
+  <si>
+    <t>18:05:15.290000</t>
+  </si>
+  <si>
+    <t>18:05:01.670000</t>
+  </si>
+  <si>
+    <t>7:43:21</t>
+  </si>
+  <si>
+    <t>7:44:15</t>
+  </si>
+  <si>
+    <t>7:45:01</t>
+  </si>
+  <si>
+    <t>Felipe Restrepo</t>
+  </si>
+  <si>
+    <t>Johan Camilo Echeverri Gil</t>
+  </si>
+  <si>
+    <t>Juan Felipe Buitrago Garcia</t>
+  </si>
+  <si>
+    <t>Santiago Holguin Álvarez</t>
+  </si>
+  <si>
+    <t>Alejandro Franco</t>
+  </si>
+  <si>
+    <t>Diego Alejandro Jaramillo Gonzalez</t>
+  </si>
+  <si>
+    <t>Daniel Loaiza López</t>
+  </si>
+  <si>
+    <t>Sebastián Carmona Sánchez</t>
+  </si>
+  <si>
+    <t>Daniel Valencia Hernandez</t>
+  </si>
+  <si>
+    <t>Jorge David Osorio Rua</t>
+  </si>
+  <si>
+    <t>Cristian Fernández Rivera</t>
+  </si>
+  <si>
+    <t>Juan José Castaño</t>
+  </si>
+  <si>
+    <t>Juan Fernando Arboleda Álvarez</t>
+  </si>
+  <si>
+    <t>Wilson Collo</t>
+  </si>
+  <si>
+    <t>Juan Pablo Lescano</t>
+  </si>
+  <si>
+    <t>Juan Carlos Galeano</t>
+  </si>
+  <si>
+    <t>TANDA SENIOR (19-29 AÑOS)</t>
+  </si>
+  <si>
+    <t>10:12:00</t>
+  </si>
+  <si>
+    <t>10:11:00</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>10:09:00</t>
+  </si>
+  <si>
+    <t>10:01:00</t>
+  </si>
+  <si>
+    <t>10:02:00</t>
+  </si>
+  <si>
+    <t>10:03:00</t>
+  </si>
+  <si>
+    <t>10:04:00</t>
+  </si>
+  <si>
+    <t>10:05:00</t>
+  </si>
+  <si>
+    <t>10:06:00</t>
+  </si>
+  <si>
+    <t>10:07:00</t>
+  </si>
+  <si>
+    <t>10:08:00</t>
+  </si>
+  <si>
+    <t>10:10:00</t>
+  </si>
+  <si>
+    <t>10:13:00</t>
+  </si>
+  <si>
+    <t>10:14:00</t>
+  </si>
+  <si>
+    <t>10:15:00</t>
+  </si>
+  <si>
+    <t>18:05:57.050000</t>
+  </si>
+  <si>
+    <t>18:05:56.580000</t>
+  </si>
+  <si>
+    <t>18:03:45.470000</t>
+  </si>
+  <si>
+    <t>7:53:57</t>
+  </si>
+  <si>
+    <t>7:54:56</t>
+  </si>
+  <si>
+    <t>8:03:45</t>
+  </si>
+  <si>
+    <t>Angelica Mazo</t>
+  </si>
+  <si>
+    <t>Johana Palacio Osorio</t>
+  </si>
+  <si>
+    <t>Catherine Restrepo Alvarez</t>
+  </si>
+  <si>
+    <t>Bibiana Restrepo</t>
+  </si>
+  <si>
     <t>Laura Aldana</t>
   </si>
   <si>
-    <t>Johana Palacio Osorio</t>
-  </si>
-  <si>
-    <t>Catherine Restrepo Alvarez</t>
-  </si>
-  <si>
-    <t>Bibiana Restrepo</t>
-  </si>
-  <si>
-    <t>Angelica Mazo</t>
-  </si>
-  <si>
     <t>Angelica Velez</t>
   </si>
   <si>
@@ -118,21 +281,21 @@
     <t xml:space="preserve">TANDA DAMAS NOVATAS </t>
   </si>
   <si>
+    <t>08:04:00</t>
+  </si>
+  <si>
+    <t>08:03:00</t>
+  </si>
+  <si>
+    <t>08:02:00</t>
+  </si>
+  <si>
+    <t>08:00:00</t>
+  </si>
+  <si>
     <t>08:01:00</t>
   </si>
   <si>
-    <t>08:03:00</t>
-  </si>
-  <si>
-    <t>08:02:00</t>
-  </si>
-  <si>
-    <t>08:00:00</t>
-  </si>
-  <si>
-    <t>08:04:00</t>
-  </si>
-  <si>
     <t>08:05:00</t>
   </si>
   <si>
@@ -196,28 +359,475 @@
     <t>08:25:00</t>
   </si>
   <si>
-    <t>00:36:48</t>
-  </si>
-  <si>
-    <t>00:58:36</t>
-  </si>
-  <si>
-    <t>00:58:35</t>
-  </si>
-  <si>
-    <t>00:58:34</t>
-  </si>
-  <si>
-    <t>16:35:48</t>
-  </si>
-  <si>
-    <t>16:55:36</t>
-  </si>
-  <si>
-    <t>16:56:35</t>
-  </si>
-  <si>
-    <t>16:58:34</t>
+    <t>17:26:46.160000</t>
+  </si>
+  <si>
+    <t>17:26:46.580000</t>
+  </si>
+  <si>
+    <t>17:26:45.720000</t>
+  </si>
+  <si>
+    <t>17:26:28.390000</t>
+  </si>
+  <si>
+    <t>9:22:46</t>
+  </si>
+  <si>
+    <t>9:23:46</t>
+  </si>
+  <si>
+    <t>9:24:45</t>
+  </si>
+  <si>
+    <t>9:26:28</t>
+  </si>
+  <si>
+    <t>Isabela Gonzalez</t>
+  </si>
+  <si>
+    <t>Jenny Campero</t>
+  </si>
+  <si>
+    <t>Dahiana García</t>
+  </si>
+  <si>
+    <t>TANDA DAMAS EXPERTAS</t>
+  </si>
+  <si>
+    <t>08:30:00</t>
+  </si>
+  <si>
+    <t>08:31:00</t>
+  </si>
+  <si>
+    <t>08:32:00</t>
+  </si>
+  <si>
+    <t>Fabricio Sacco Muñoz</t>
+  </si>
+  <si>
+    <t>Orlando Montoya Cardona</t>
+  </si>
+  <si>
+    <t>Iván Cano Rodriguez</t>
+  </si>
+  <si>
+    <t>Juan Pablo Castrillón</t>
+  </si>
+  <si>
+    <t>Jaime De Jesus Gallego Gomez</t>
+  </si>
+  <si>
+    <t>Ruben Dario Restrepo</t>
+  </si>
+  <si>
+    <t>Fernando Parra</t>
+  </si>
+  <si>
+    <t>TANDA MASTER C (50 AÑOS EN ADELANTE)</t>
+  </si>
+  <si>
+    <t>08:35:00</t>
+  </si>
+  <si>
+    <t>08:36:00</t>
+  </si>
+  <si>
+    <t>08:37:00</t>
+  </si>
+  <si>
+    <t>08:38:00</t>
+  </si>
+  <si>
+    <t>08:39:00</t>
+  </si>
+  <si>
+    <t>08:40:00</t>
+  </si>
+  <si>
+    <t>08:41:00</t>
+  </si>
+  <si>
+    <t>Edgar Alexander Mosquera Cuello</t>
+  </si>
+  <si>
+    <t>Ferney Acevedo Correa</t>
+  </si>
+  <si>
+    <t>Fredy Alberto Acevedo Correa</t>
+  </si>
+  <si>
+    <t>Albeiro Arias</t>
+  </si>
+  <si>
+    <t>Sergio Andrés Echeverri Ceballos</t>
+  </si>
+  <si>
+    <t>Alejandro Bedoya Vasquez</t>
+  </si>
+  <si>
+    <t>Victor Manuel Caro Echeverri</t>
+  </si>
+  <si>
+    <t>Estiven Vélez Ortiz</t>
+  </si>
+  <si>
+    <t>Adrian Felipe Flórez Martínez</t>
+  </si>
+  <si>
+    <t>Luis Mauricio López Salazar</t>
+  </si>
+  <si>
+    <t>Julian Alonso Arango Olaya</t>
+  </si>
+  <si>
+    <t>Julian David Gutiérrez Moreno</t>
+  </si>
+  <si>
+    <t>Jaime David Medina Múnera</t>
+  </si>
+  <si>
+    <t>Juan Carlos Herrera Naranjo</t>
+  </si>
+  <si>
+    <t>John Restrepo</t>
+  </si>
+  <si>
+    <t>Edwin Agudelo Urrego</t>
+  </si>
+  <si>
+    <t>Luis Alejandro López</t>
+  </si>
+  <si>
+    <t>Julian Ortiz Escobar</t>
+  </si>
+  <si>
+    <t>Elkin Dario Murillo Alzate</t>
+  </si>
+  <si>
+    <t>Juan Camilo Zapata</t>
+  </si>
+  <si>
+    <t>Juan José Henao Aristizábal</t>
+  </si>
+  <si>
+    <t>Hugo Osorio Patiño</t>
+  </si>
+  <si>
+    <t>Sergio Jaramillo Castro</t>
+  </si>
+  <si>
+    <t>Andrés Cadavid</t>
+  </si>
+  <si>
+    <t>Juan Daniel Yepez Vahos</t>
+  </si>
+  <si>
+    <t>Yeison Ferney Ospina Guerra</t>
+  </si>
+  <si>
+    <t>Osman Soto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan Felipe Bueno Rincón </t>
+  </si>
+  <si>
+    <t>Víctor Mejia Martinez</t>
+  </si>
+  <si>
+    <t>Diego Santa</t>
+  </si>
+  <si>
+    <t>Jonathan Fernández Pérez</t>
+  </si>
+  <si>
+    <t>TANDA NOVATOS</t>
+  </si>
+  <si>
+    <t>08:45:00</t>
+  </si>
+  <si>
+    <t>08:46:00</t>
+  </si>
+  <si>
+    <t>08:47:00</t>
+  </si>
+  <si>
+    <t>08:48:00</t>
+  </si>
+  <si>
+    <t>08:49:00</t>
+  </si>
+  <si>
+    <t>08:50:00</t>
+  </si>
+  <si>
+    <t>08:51:00</t>
+  </si>
+  <si>
+    <t>08:52:00</t>
+  </si>
+  <si>
+    <t>08:53:00</t>
+  </si>
+  <si>
+    <t>08:54:00</t>
+  </si>
+  <si>
+    <t>08:55:00</t>
+  </si>
+  <si>
+    <t>08:56:00</t>
+  </si>
+  <si>
+    <t>08:57:00</t>
+  </si>
+  <si>
+    <t>08:58:00</t>
+  </si>
+  <si>
+    <t>08:59:00</t>
+  </si>
+  <si>
+    <t>09:00:00</t>
+  </si>
+  <si>
+    <t>09:01:00</t>
+  </si>
+  <si>
+    <t>09:02:00</t>
+  </si>
+  <si>
+    <t>09:03:00</t>
+  </si>
+  <si>
+    <t>09:04:00</t>
+  </si>
+  <si>
+    <t>09:05:00</t>
+  </si>
+  <si>
+    <t>09:06:00</t>
+  </si>
+  <si>
+    <t>09:07:00</t>
+  </si>
+  <si>
+    <t>09:08:00</t>
+  </si>
+  <si>
+    <t>09:09:00</t>
+  </si>
+  <si>
+    <t>09:10:00</t>
+  </si>
+  <si>
+    <t>09:11:00</t>
+  </si>
+  <si>
+    <t>09:12:00</t>
+  </si>
+  <si>
+    <t>09:13:00</t>
+  </si>
+  <si>
+    <t>09:14:00</t>
+  </si>
+  <si>
+    <t>09:15:00</t>
+  </si>
+  <si>
+    <t>Andres Mauricio Vargas Hernandez</t>
+  </si>
+  <si>
+    <t>José Agustín Castillo Moreno</t>
+  </si>
+  <si>
+    <t>Jhony Jimenez</t>
+  </si>
+  <si>
+    <t>Jairo Gallego Castaño</t>
+  </si>
+  <si>
+    <t>Carlos Arroyave</t>
+  </si>
+  <si>
+    <t>Juan Diego Mejía Vallejo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauricio González </t>
+  </si>
+  <si>
+    <t>TANDA MASTER B (40-49 AÑOS)</t>
+  </si>
+  <si>
+    <t>09:20:00</t>
+  </si>
+  <si>
+    <t>09:21:00</t>
+  </si>
+  <si>
+    <t>09:22:00</t>
+  </si>
+  <si>
+    <t>09:23:00</t>
+  </si>
+  <si>
+    <t>09:24:00</t>
+  </si>
+  <si>
+    <t>09:25:00</t>
+  </si>
+  <si>
+    <t>09:26:00</t>
+  </si>
+  <si>
+    <t>Carlos Mario Caicedo Arboleda</t>
+  </si>
+  <si>
+    <t>Juan Carlos López Molina</t>
+  </si>
+  <si>
+    <t>Juan David Gallego Arroyave</t>
+  </si>
+  <si>
+    <t>Carlos A. Piedrahita E.</t>
+  </si>
+  <si>
+    <t>Norbey Araque</t>
+  </si>
+  <si>
+    <t>Jorge Alejandro Arévalo Cardona</t>
+  </si>
+  <si>
+    <t>Juan Alberto Munera Alzate</t>
+  </si>
+  <si>
+    <t>Jesús Andrés Hincapié</t>
+  </si>
+  <si>
+    <t>Julian Correa</t>
+  </si>
+  <si>
+    <t>Juan Sebastian Alcaraz Vega</t>
+  </si>
+  <si>
+    <t>Diego Ruiz</t>
+  </si>
+  <si>
+    <t>Andres Montilla</t>
+  </si>
+  <si>
+    <t>Jaime Alberto Zuluaga Toro</t>
+  </si>
+  <si>
+    <t>Daniel López Valencia</t>
+  </si>
+  <si>
+    <t>Jesús Garzón</t>
+  </si>
+  <si>
+    <t>Javier Darío Posada Agudelo</t>
+  </si>
+  <si>
+    <t>Juan José Vélez Ortega</t>
+  </si>
+  <si>
+    <t>Diego Alexander Ocampo Betancur</t>
+  </si>
+  <si>
+    <t>Julian Fernandez Giraldo</t>
+  </si>
+  <si>
+    <t>David Alonso Ramirez Parra</t>
+  </si>
+  <si>
+    <t>Oscar Guerrero</t>
+  </si>
+  <si>
+    <t>Edwin Orlando Murillo Torres</t>
+  </si>
+  <si>
+    <t>Hermes Oquendo</t>
+  </si>
+  <si>
+    <t>Javier Castillo</t>
+  </si>
+  <si>
+    <t>TANDA MASTER A (30-39 AÑOS)</t>
+  </si>
+  <si>
+    <t>09:30:00</t>
+  </si>
+  <si>
+    <t>09:31:00</t>
+  </si>
+  <si>
+    <t>09:32:00</t>
+  </si>
+  <si>
+    <t>09:33:00</t>
+  </si>
+  <si>
+    <t>09:34:00</t>
+  </si>
+  <si>
+    <t>09:35:00</t>
+  </si>
+  <si>
+    <t>09:36:00</t>
+  </si>
+  <si>
+    <t>09:37:00</t>
+  </si>
+  <si>
+    <t>09:38:00</t>
+  </si>
+  <si>
+    <t>09:39:00</t>
+  </si>
+  <si>
+    <t>09:40:00</t>
+  </si>
+  <si>
+    <t>09:41:00</t>
+  </si>
+  <si>
+    <t>09:42:00</t>
+  </si>
+  <si>
+    <t>09:43:00</t>
+  </si>
+  <si>
+    <t>09:44:00</t>
+  </si>
+  <si>
+    <t>09:45:00</t>
+  </si>
+  <si>
+    <t>09:46:00</t>
+  </si>
+  <si>
+    <t>09:47:00</t>
+  </si>
+  <si>
+    <t>09:48:00</t>
+  </si>
+  <si>
+    <t>09:49:00</t>
+  </si>
+  <si>
+    <t>09:50:00</t>
+  </si>
+  <si>
+    <t>09:51:00</t>
+  </si>
+  <si>
+    <t>09:52:00</t>
+  </si>
+  <si>
+    <t>09:53:00</t>
   </si>
 </sst>
 </file>
@@ -575,7 +1185,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -609,19 +1219,19 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -632,19 +1242,19 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -655,42 +1265,434 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>62</v>
       </c>
       <c r="B5">
         <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -698,310 +1700,1498 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B6">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B14">
         <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="B15">
         <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B16">
         <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B17">
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B19">
         <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="B20">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="B21">
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="B22">
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="B23">
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="B24">
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="B25">
         <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="B26">
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B27">
         <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2">
+        <v>176</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>171</v>
+      </c>
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4">
+        <v>177</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5">
+        <v>178</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <v>179</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <v>174</v>
+      </c>
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>175</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3">
+        <v>236</v>
+      </c>
+      <c r="C3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4">
+        <v>237</v>
+      </c>
+      <c r="C4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5">
+        <v>181</v>
+      </c>
+      <c r="C5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7">
+        <v>238</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8">
+        <v>198</v>
+      </c>
+      <c r="C8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9">
+        <v>187</v>
+      </c>
+      <c r="C9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10">
+        <v>239</v>
+      </c>
+      <c r="C10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11">
+        <v>240</v>
+      </c>
+      <c r="C11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12">
+        <v>218</v>
+      </c>
+      <c r="C12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13">
+        <v>241</v>
+      </c>
+      <c r="C13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14">
+        <v>242</v>
+      </c>
+      <c r="C14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15">
+        <v>243</v>
+      </c>
+      <c r="C15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16">
+        <v>194</v>
+      </c>
+      <c r="C16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17">
+        <v>191</v>
+      </c>
+      <c r="C17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18">
+        <v>244</v>
+      </c>
+      <c r="C18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19">
+        <v>245</v>
+      </c>
+      <c r="C19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20">
+        <v>193</v>
+      </c>
+      <c r="C20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21">
+        <v>246</v>
+      </c>
+      <c r="C21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22">
+        <v>203</v>
+      </c>
+      <c r="C22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23">
+        <v>247</v>
+      </c>
+      <c r="C23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24">
+        <v>248</v>
+      </c>
+      <c r="C24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25">
+        <v>249</v>
+      </c>
+      <c r="C25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26">
+        <v>199</v>
+      </c>
+      <c r="C26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27">
+        <v>250</v>
+      </c>
+      <c r="C27" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28">
+        <v>122</v>
+      </c>
+      <c r="C28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29">
+        <v>222</v>
+      </c>
+      <c r="C29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30">
+        <v>228</v>
+      </c>
+      <c r="C30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31">
+        <v>159</v>
+      </c>
+      <c r="C31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>172</v>
+      </c>
+      <c r="B32">
+        <v>169</v>
+      </c>
+      <c r="C32" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2">
+        <v>158</v>
+      </c>
+      <c r="C2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3">
+        <v>155</v>
+      </c>
+      <c r="C3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4">
+        <v>156</v>
+      </c>
+      <c r="C4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5">
+        <v>160</v>
+      </c>
+      <c r="C5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6">
+        <v>154</v>
+      </c>
+      <c r="C6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7">
+        <v>161</v>
+      </c>
+      <c r="C7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8">
+        <v>140</v>
+      </c>
+      <c r="C8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11">
+        <v>136</v>
+      </c>
+      <c r="C11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B12">
+        <v>114</v>
+      </c>
+      <c r="C12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B13">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B14">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15">
+        <v>139</v>
+      </c>
+      <c r="C15" t="s">
+        <v>244</v>
+      </c>
+      <c r="D15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B16">
+        <v>162</v>
+      </c>
+      <c r="C16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B17">
+        <v>163</v>
+      </c>
+      <c r="C17" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18">
+        <v>111</v>
+      </c>
+      <c r="C18" t="s">
+        <v>244</v>
+      </c>
+      <c r="D18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19">
+        <v>164</v>
+      </c>
+      <c r="C19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>238</v>
+      </c>
+      <c r="B20">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B21">
+        <v>165</v>
+      </c>
+      <c r="C21" t="s">
+        <v>244</v>
+      </c>
+      <c r="D21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22">
+        <v>166</v>
+      </c>
+      <c r="C22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D22" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>241</v>
+      </c>
+      <c r="B23">
+        <v>118</v>
+      </c>
+      <c r="C23" t="s">
+        <v>244</v>
+      </c>
+      <c r="D23" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24">
+        <v>167</v>
+      </c>
+      <c r="C24" t="s">
+        <v>244</v>
+      </c>
+      <c r="D24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B25">
+        <v>168</v>
+      </c>
+      <c r="C25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>